<commit_message>
ensure all data used in Corelogic
</commit_message>
<xml_diff>
--- a/data-raw/abs/payrolls/6160055001_DO006.xlsx
+++ b/data-raw/abs/payrolls/6160055001_DO006.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp\absdfs\workgroup\LMS\STP Covid-19 project\Dissemination\Week ending 13 February 2021\IPE materials\Downloads\Thursday\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp\absdfs\workgroup\LMS\STP Covid-19 project\Dissemination\Week ending 27 February 2021\IPE materials\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931B9258-73EB-4381-8909-42365199C3B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1C4474-490C-4CF9-A37F-5E6E4D5B5413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="120">
   <si>
     <t>10. J-Information media &amp; telecommunications</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Industry</t>
-  </si>
-  <si>
-    <t>Sub-division</t>
   </si>
   <si>
     <t>01. Agriculture</t>
@@ -395,10 +392,16 @@
     <t>© Commonwealth of Australia 2021</t>
   </si>
   <si>
-    <t>Week ending Saturday 13 February 2021</t>
+    <t>NA</t>
   </si>
   <si>
-    <t>Released at 11.30am (Canberra time) 4 March 2021</t>
+    <t>Week ending Saturday 27 February 2021</t>
+  </si>
+  <si>
+    <t>Released at 11.30am (Canberra time) 16 March 2021</t>
+  </si>
+  <si>
+    <t>Subdivision</t>
   </si>
 </sst>
 </file>
@@ -550,7 +553,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection hidden="1"/>
@@ -615,6 +618,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1053,7 +1059,7 @@
   <dimension ref="A1:BC19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection sqref="A1:B1"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1379,7 +1385,7 @@
     </row>
     <row r="2" spans="1:55" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:55" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1404,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:55" x14ac:dyDescent="0.25">
@@ -1444,24 +1450,24 @@
       <c r="C15" s="21"/>
     </row>
     <row r="16" spans="1:55" ht="22.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="27"/>
+      <c r="C16" s="28"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="21"/>
       <c r="C18" s="21"/>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C19" s="28"/>
+      <c r="B19" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C19" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1584,7 +1590,7 @@
     </row>
     <row r="2" spans="1:79" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1913,7 +1919,7 @@
         <v>26</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>27</v>
+        <v>119</v>
       </c>
       <c r="C6" s="25">
         <v>43834</v>
@@ -2092,8 +2098,12 @@
       <c r="BI6" s="25">
         <v>44240</v>
       </c>
-      <c r="BJ6" s="25"/>
-      <c r="BK6" s="25"/>
+      <c r="BJ6" s="25">
+        <v>44247</v>
+      </c>
+      <c r="BK6" s="25">
+        <v>44254</v>
+      </c>
       <c r="BL6" s="25"/>
       <c r="BM6" s="25"/>
       <c r="BN6" s="25"/>
@@ -2115,7 +2125,7 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="26">
         <v>92.74</v>
@@ -2294,8 +2304,12 @@
       <c r="BI7" s="26">
         <v>95.6</v>
       </c>
-      <c r="BJ7" s="26"/>
-      <c r="BK7" s="26"/>
+      <c r="BJ7" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK7" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL7" s="26"/>
       <c r="BM7" s="26"/>
       <c r="BN7" s="26"/>
@@ -2318,7 +2332,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" s="26">
         <v>93.83</v>
@@ -2497,8 +2511,12 @@
       <c r="BI8" s="26">
         <v>100.02</v>
       </c>
-      <c r="BJ8" s="26"/>
-      <c r="BK8" s="26"/>
+      <c r="BJ8" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK8" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL8" s="26"/>
       <c r="BM8" s="26"/>
       <c r="BN8" s="26"/>
@@ -2521,7 +2539,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="26">
         <v>91.48</v>
@@ -2700,8 +2718,12 @@
       <c r="BI9" s="26">
         <v>89</v>
       </c>
-      <c r="BJ9" s="26"/>
-      <c r="BK9" s="26"/>
+      <c r="BJ9" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK9" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL9" s="26"/>
       <c r="BM9" s="26"/>
       <c r="BN9" s="26"/>
@@ -2724,7 +2746,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C10" s="26">
         <v>92.24</v>
@@ -2903,8 +2925,12 @@
       <c r="BI10" s="26">
         <v>85.73</v>
       </c>
-      <c r="BJ10" s="26"/>
-      <c r="BK10" s="26"/>
+      <c r="BJ10" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK10" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL10" s="26"/>
       <c r="BM10" s="26"/>
       <c r="BN10" s="26"/>
@@ -2927,7 +2953,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="26">
         <v>82.57</v>
@@ -3106,8 +3132,12 @@
       <c r="BI11" s="26">
         <v>96.5</v>
       </c>
-      <c r="BJ11" s="26"/>
-      <c r="BK11" s="26"/>
+      <c r="BJ11" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK11" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL11" s="26"/>
       <c r="BM11" s="26"/>
       <c r="BN11" s="26"/>
@@ -3130,7 +3160,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="26">
         <v>100.15</v>
@@ -3309,8 +3339,12 @@
       <c r="BI12" s="26">
         <v>97.25</v>
       </c>
-      <c r="BJ12" s="26"/>
-      <c r="BK12" s="26"/>
+      <c r="BJ12" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK12" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL12" s="26"/>
       <c r="BM12" s="26"/>
       <c r="BN12" s="26"/>
@@ -3333,7 +3367,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="26">
         <v>96</v>
@@ -3512,8 +3546,12 @@
       <c r="BI13" s="26">
         <v>91.24</v>
       </c>
-      <c r="BJ13" s="26"/>
-      <c r="BK13" s="26"/>
+      <c r="BJ13" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK13" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL13" s="26"/>
       <c r="BM13" s="26"/>
       <c r="BN13" s="26"/>
@@ -3536,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="26">
         <v>96.02</v>
@@ -3715,8 +3753,12 @@
       <c r="BI14" s="26">
         <v>96.59</v>
       </c>
-      <c r="BJ14" s="26"/>
-      <c r="BK14" s="26"/>
+      <c r="BJ14" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK14" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL14" s="26"/>
       <c r="BM14" s="26"/>
       <c r="BN14" s="26"/>
@@ -3739,7 +3781,7 @@
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="26">
         <v>90.36</v>
@@ -3918,8 +3960,12 @@
       <c r="BI15" s="26">
         <v>101.61</v>
       </c>
-      <c r="BJ15" s="26"/>
-      <c r="BK15" s="26"/>
+      <c r="BJ15" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK15" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL15" s="26"/>
       <c r="BM15" s="26"/>
       <c r="BN15" s="26"/>
@@ -3942,7 +3988,7 @@
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C16" s="26">
         <v>94.69</v>
@@ -4121,8 +4167,12 @@
       <c r="BI16" s="26">
         <v>108.42</v>
       </c>
-      <c r="BJ16" s="26"/>
-      <c r="BK16" s="26"/>
+      <c r="BJ16" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK16" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL16" s="26"/>
       <c r="BM16" s="26"/>
       <c r="BN16" s="26"/>
@@ -4145,7 +4195,7 @@
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="26">
         <v>94.06</v>
@@ -4324,8 +4374,12 @@
       <c r="BI17" s="26">
         <v>94.25</v>
       </c>
-      <c r="BJ17" s="26"/>
-      <c r="BK17" s="26"/>
+      <c r="BJ17" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK17" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL17" s="26"/>
       <c r="BM17" s="26"/>
       <c r="BN17" s="26"/>
@@ -4348,7 +4402,7 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="26">
         <v>93.16</v>
@@ -4527,8 +4581,12 @@
       <c r="BI18" s="26">
         <v>98.23</v>
       </c>
-      <c r="BJ18" s="26"/>
-      <c r="BK18" s="26"/>
+      <c r="BJ18" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK18" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL18" s="26"/>
       <c r="BM18" s="26"/>
       <c r="BN18" s="26"/>
@@ -4551,7 +4609,7 @@
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="26">
         <v>81.93</v>
@@ -4730,8 +4788,12 @@
       <c r="BI19" s="26">
         <v>97.59</v>
       </c>
-      <c r="BJ19" s="26"/>
-      <c r="BK19" s="26"/>
+      <c r="BJ19" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK19" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL19" s="26"/>
       <c r="BM19" s="26"/>
       <c r="BN19" s="26"/>
@@ -4754,7 +4816,7 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="26">
         <v>81.77</v>
@@ -4933,8 +4995,12 @@
       <c r="BI20" s="26">
         <v>96.71</v>
       </c>
-      <c r="BJ20" s="26"/>
-      <c r="BK20" s="26"/>
+      <c r="BJ20" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK20" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL20" s="26"/>
       <c r="BM20" s="26"/>
       <c r="BN20" s="26"/>
@@ -4957,7 +5023,7 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="26">
         <v>95.41</v>
@@ -5136,8 +5202,12 @@
       <c r="BI21" s="26">
         <v>92.18</v>
       </c>
-      <c r="BJ21" s="26"/>
-      <c r="BK21" s="26"/>
+      <c r="BJ21" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK21" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL21" s="26"/>
       <c r="BM21" s="26"/>
       <c r="BN21" s="26"/>
@@ -5160,7 +5230,7 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C22" s="26">
         <v>91.59</v>
@@ -5339,8 +5409,12 @@
       <c r="BI22" s="26">
         <v>92.69</v>
       </c>
-      <c r="BJ22" s="26"/>
-      <c r="BK22" s="26"/>
+      <c r="BJ22" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK22" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL22" s="26"/>
       <c r="BM22" s="26"/>
       <c r="BN22" s="26"/>
@@ -5363,7 +5437,7 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="26">
         <v>94.74</v>
@@ -5542,8 +5616,12 @@
       <c r="BI23" s="26">
         <v>91.78</v>
       </c>
-      <c r="BJ23" s="26"/>
-      <c r="BK23" s="26"/>
+      <c r="BJ23" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK23" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL23" s="26"/>
       <c r="BM23" s="26"/>
       <c r="BN23" s="26"/>
@@ -5566,7 +5644,7 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C24" s="26">
         <v>97.18</v>
@@ -5745,8 +5823,12 @@
       <c r="BI24" s="26">
         <v>107.06</v>
       </c>
-      <c r="BJ24" s="26"/>
-      <c r="BK24" s="26"/>
+      <c r="BJ24" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK24" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL24" s="26"/>
       <c r="BM24" s="26"/>
       <c r="BN24" s="26"/>
@@ -5769,7 +5851,7 @@
         <v>12</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" s="26">
         <v>88.58</v>
@@ -5948,8 +6030,12 @@
       <c r="BI25" s="26">
         <v>100.71</v>
       </c>
-      <c r="BJ25" s="26"/>
-      <c r="BK25" s="26"/>
+      <c r="BJ25" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK25" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL25" s="26"/>
       <c r="BM25" s="26"/>
       <c r="BN25" s="26"/>
@@ -5972,7 +6058,7 @@
         <v>12</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C26" s="26">
         <v>90.9</v>
@@ -6151,8 +6237,12 @@
       <c r="BI26" s="26">
         <v>93.04</v>
       </c>
-      <c r="BJ26" s="26"/>
-      <c r="BK26" s="26"/>
+      <c r="BJ26" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK26" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL26" s="26"/>
       <c r="BM26" s="26"/>
       <c r="BN26" s="26"/>
@@ -6175,7 +6265,7 @@
         <v>12</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="26">
         <v>93.24</v>
@@ -6354,8 +6444,12 @@
       <c r="BI27" s="26">
         <v>98.59</v>
       </c>
-      <c r="BJ27" s="26"/>
-      <c r="BK27" s="26"/>
+      <c r="BJ27" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK27" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL27" s="26"/>
       <c r="BM27" s="26"/>
       <c r="BN27" s="26"/>
@@ -6378,7 +6472,7 @@
         <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" s="26">
         <v>85</v>
@@ -6557,8 +6651,12 @@
       <c r="BI28" s="26">
         <v>95.07</v>
       </c>
-      <c r="BJ28" s="26"/>
-      <c r="BK28" s="26"/>
+      <c r="BJ28" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK28" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL28" s="26"/>
       <c r="BM28" s="26"/>
       <c r="BN28" s="26"/>
@@ -6581,7 +6679,7 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="26">
         <v>91.63</v>
@@ -6760,8 +6858,12 @@
       <c r="BI29" s="26">
         <v>95.74</v>
       </c>
-      <c r="BJ29" s="26"/>
-      <c r="BK29" s="26"/>
+      <c r="BJ29" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK29" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL29" s="26"/>
       <c r="BM29" s="26"/>
       <c r="BN29" s="26"/>
@@ -6784,7 +6886,7 @@
         <v>12</v>
       </c>
       <c r="B30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="26">
         <v>92.35</v>
@@ -6963,8 +7065,12 @@
       <c r="BI30" s="26">
         <v>98.3</v>
       </c>
-      <c r="BJ30" s="26"/>
-      <c r="BK30" s="26"/>
+      <c r="BJ30" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK30" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL30" s="26"/>
       <c r="BM30" s="26"/>
       <c r="BN30" s="26"/>
@@ -6987,7 +7093,7 @@
         <v>12</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" s="26">
         <v>84.26</v>
@@ -7166,8 +7272,12 @@
       <c r="BI31" s="26">
         <v>95.23</v>
       </c>
-      <c r="BJ31" s="26"/>
-      <c r="BK31" s="26"/>
+      <c r="BJ31" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK31" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL31" s="26"/>
       <c r="BM31" s="26"/>
       <c r="BN31" s="26"/>
@@ -7190,7 +7300,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" s="26">
         <v>95.26</v>
@@ -7369,8 +7479,12 @@
       <c r="BI32" s="26">
         <v>102.81</v>
       </c>
-      <c r="BJ32" s="26"/>
-      <c r="BK32" s="26"/>
+      <c r="BJ32" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK32" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL32" s="26"/>
       <c r="BM32" s="26"/>
       <c r="BN32" s="26"/>
@@ -7393,7 +7507,7 @@
         <v>13</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" s="26">
         <v>83.53</v>
@@ -7572,8 +7686,12 @@
       <c r="BI33" s="26">
         <v>112.73</v>
       </c>
-      <c r="BJ33" s="26"/>
-      <c r="BK33" s="26"/>
+      <c r="BJ33" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK33" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL33" s="26"/>
       <c r="BM33" s="26"/>
       <c r="BN33" s="26"/>
@@ -7596,7 +7714,7 @@
         <v>13</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" s="26">
         <v>96.3</v>
@@ -7775,8 +7893,12 @@
       <c r="BI34" s="26">
         <v>102.58</v>
       </c>
-      <c r="BJ34" s="26"/>
-      <c r="BK34" s="26"/>
+      <c r="BJ34" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK34" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL34" s="26"/>
       <c r="BM34" s="26"/>
       <c r="BN34" s="26"/>
@@ -7799,7 +7921,7 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="26">
         <v>89.16</v>
@@ -7978,8 +8100,12 @@
       <c r="BI35" s="26">
         <v>98.31</v>
       </c>
-      <c r="BJ35" s="26"/>
-      <c r="BK35" s="26"/>
+      <c r="BJ35" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK35" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL35" s="26"/>
       <c r="BM35" s="26"/>
       <c r="BN35" s="26"/>
@@ -8002,7 +8128,7 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="26">
         <v>86.86</v>
@@ -8181,8 +8307,12 @@
       <c r="BI36" s="26">
         <v>99.04</v>
       </c>
-      <c r="BJ36" s="26"/>
-      <c r="BK36" s="26"/>
+      <c r="BJ36" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK36" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL36" s="26"/>
       <c r="BM36" s="26"/>
       <c r="BN36" s="26"/>
@@ -8205,7 +8335,7 @@
         <v>14</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C37" s="26">
         <v>89.81</v>
@@ -8384,8 +8514,12 @@
       <c r="BI37" s="26">
         <v>88</v>
       </c>
-      <c r="BJ37" s="26"/>
-      <c r="BK37" s="26"/>
+      <c r="BJ37" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK37" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL37" s="26"/>
       <c r="BM37" s="26"/>
       <c r="BN37" s="26"/>
@@ -8408,7 +8542,7 @@
         <v>14</v>
       </c>
       <c r="B38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="26">
         <v>84.33</v>
@@ -8587,8 +8721,12 @@
       <c r="BI38" s="26">
         <v>95.27</v>
       </c>
-      <c r="BJ38" s="26"/>
-      <c r="BK38" s="26"/>
+      <c r="BJ38" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK38" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL38" s="26"/>
       <c r="BM38" s="26"/>
       <c r="BN38" s="26"/>
@@ -8611,7 +8749,7 @@
         <v>15</v>
       </c>
       <c r="B39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="26">
         <v>93.48</v>
@@ -8790,8 +8928,12 @@
       <c r="BI39" s="26">
         <v>95.81</v>
       </c>
-      <c r="BJ39" s="26"/>
-      <c r="BK39" s="26"/>
+      <c r="BJ39" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK39" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL39" s="26"/>
       <c r="BM39" s="26"/>
       <c r="BN39" s="26"/>
@@ -8814,7 +8956,7 @@
         <v>15</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C40" s="26">
         <v>96.27</v>
@@ -8993,8 +9135,12 @@
       <c r="BI40" s="26">
         <v>98.22</v>
       </c>
-      <c r="BJ40" s="26"/>
-      <c r="BK40" s="26"/>
+      <c r="BJ40" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK40" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL40" s="26"/>
       <c r="BM40" s="26"/>
       <c r="BN40" s="26"/>
@@ -9017,7 +9163,7 @@
         <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="26">
         <v>96.58</v>
@@ -9196,8 +9342,12 @@
       <c r="BI41" s="26">
         <v>93.32</v>
       </c>
-      <c r="BJ41" s="26"/>
-      <c r="BK41" s="26"/>
+      <c r="BJ41" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK41" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL41" s="26"/>
       <c r="BM41" s="26"/>
       <c r="BN41" s="26"/>
@@ -9220,7 +9370,7 @@
         <v>15</v>
       </c>
       <c r="B42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C42" s="26">
         <v>94.95</v>
@@ -9399,8 +9549,12 @@
       <c r="BI42" s="26">
         <v>95.16</v>
       </c>
-      <c r="BJ42" s="26"/>
-      <c r="BK42" s="26"/>
+      <c r="BJ42" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK42" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL42" s="26"/>
       <c r="BM42" s="26"/>
       <c r="BN42" s="26"/>
@@ -9423,7 +9577,7 @@
         <v>15</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C43" s="26">
         <v>96.02</v>
@@ -9602,8 +9756,12 @@
       <c r="BI43" s="26">
         <v>95.97</v>
       </c>
-      <c r="BJ43" s="26"/>
-      <c r="BK43" s="26"/>
+      <c r="BJ43" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK43" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL43" s="26"/>
       <c r="BM43" s="26"/>
       <c r="BN43" s="26"/>
@@ -9626,7 +9784,7 @@
         <v>15</v>
       </c>
       <c r="B44" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C44" s="26">
         <v>86.81</v>
@@ -9805,8 +9963,12 @@
       <c r="BI44" s="26">
         <v>101.1</v>
       </c>
-      <c r="BJ44" s="26"/>
-      <c r="BK44" s="26"/>
+      <c r="BJ44" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK44" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL44" s="26"/>
       <c r="BM44" s="26"/>
       <c r="BN44" s="26"/>
@@ -9829,7 +9991,7 @@
         <v>16</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C45" s="26">
         <v>102.02</v>
@@ -10008,8 +10170,12 @@
       <c r="BI45" s="26">
         <v>98</v>
       </c>
-      <c r="BJ45" s="26"/>
-      <c r="BK45" s="26"/>
+      <c r="BJ45" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK45" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL45" s="26"/>
       <c r="BM45" s="26"/>
       <c r="BN45" s="26"/>
@@ -10032,7 +10198,7 @@
         <v>16</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="26">
         <v>97.62</v>
@@ -10211,8 +10377,12 @@
       <c r="BI46" s="26">
         <v>106.43</v>
       </c>
-      <c r="BJ46" s="26"/>
-      <c r="BK46" s="26"/>
+      <c r="BJ46" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK46" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL46" s="26"/>
       <c r="BM46" s="26"/>
       <c r="BN46" s="26"/>
@@ -10235,7 +10405,7 @@
         <v>16</v>
       </c>
       <c r="B47" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C47" s="26">
         <v>97.12</v>
@@ -10414,8 +10584,12 @@
       <c r="BI47" s="26">
         <v>97.68</v>
       </c>
-      <c r="BJ47" s="26"/>
-      <c r="BK47" s="26"/>
+      <c r="BJ47" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK47" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL47" s="26"/>
       <c r="BM47" s="26"/>
       <c r="BN47" s="26"/>
@@ -10438,7 +10612,7 @@
         <v>16</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C48" s="26">
         <v>102.87</v>
@@ -10617,8 +10791,12 @@
       <c r="BI48" s="26">
         <v>100.04</v>
       </c>
-      <c r="BJ48" s="26"/>
-      <c r="BK48" s="26"/>
+      <c r="BJ48" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK48" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL48" s="26"/>
       <c r="BM48" s="26"/>
       <c r="BN48" s="26"/>
@@ -10641,7 +10819,7 @@
         <v>16</v>
       </c>
       <c r="B49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C49" s="26">
         <v>92.81</v>
@@ -10820,8 +10998,12 @@
       <c r="BI49" s="26">
         <v>99.93</v>
       </c>
-      <c r="BJ49" s="26"/>
-      <c r="BK49" s="26"/>
+      <c r="BJ49" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK49" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL49" s="26"/>
       <c r="BM49" s="26"/>
       <c r="BN49" s="26"/>
@@ -10844,7 +11026,7 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="26">
         <v>96.6</v>
@@ -11023,8 +11205,12 @@
       <c r="BI50" s="26">
         <v>83.6</v>
       </c>
-      <c r="BJ50" s="26"/>
-      <c r="BK50" s="26"/>
+      <c r="BJ50" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK50" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL50" s="26"/>
       <c r="BM50" s="26"/>
       <c r="BN50" s="26"/>
@@ -11047,7 +11233,7 @@
         <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C51" s="26">
         <v>93.43</v>
@@ -11226,8 +11412,12 @@
       <c r="BI51" s="26">
         <v>88.17</v>
       </c>
-      <c r="BJ51" s="26"/>
-      <c r="BK51" s="26"/>
+      <c r="BJ51" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK51" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL51" s="26"/>
       <c r="BM51" s="26"/>
       <c r="BN51" s="26"/>
@@ -11250,7 +11440,7 @@
         <v>18</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C52" s="26">
         <v>90.64</v>
@@ -11429,8 +11619,12 @@
       <c r="BI52" s="26">
         <v>95.49</v>
       </c>
-      <c r="BJ52" s="26"/>
-      <c r="BK52" s="26"/>
+      <c r="BJ52" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK52" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL52" s="26"/>
       <c r="BM52" s="26"/>
       <c r="BN52" s="26"/>
@@ -11453,7 +11647,7 @@
         <v>18</v>
       </c>
       <c r="B53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C53" s="26">
         <v>98.99</v>
@@ -11632,8 +11826,12 @@
       <c r="BI53" s="26">
         <v>102.83</v>
       </c>
-      <c r="BJ53" s="26"/>
-      <c r="BK53" s="26"/>
+      <c r="BJ53" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK53" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL53" s="26"/>
       <c r="BM53" s="26"/>
       <c r="BN53" s="26"/>
@@ -11656,7 +11854,7 @@
         <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C54" s="26">
         <v>97.91</v>
@@ -11835,8 +12033,12 @@
       <c r="BI54" s="26">
         <v>85.74</v>
       </c>
-      <c r="BJ54" s="26"/>
-      <c r="BK54" s="26"/>
+      <c r="BJ54" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK54" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL54" s="26"/>
       <c r="BM54" s="26"/>
       <c r="BN54" s="26"/>
@@ -11859,7 +12061,7 @@
         <v>18</v>
       </c>
       <c r="B55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C55" s="26">
         <v>99.43</v>
@@ -12038,8 +12240,12 @@
       <c r="BI55" s="26">
         <v>80.22</v>
       </c>
-      <c r="BJ55" s="26"/>
-      <c r="BK55" s="26"/>
+      <c r="BJ55" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK55" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL55" s="26"/>
       <c r="BM55" s="26"/>
       <c r="BN55" s="26"/>
@@ -12062,7 +12268,7 @@
         <v>18</v>
       </c>
       <c r="B56" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C56" s="26">
         <v>98.72</v>
@@ -12241,8 +12447,12 @@
       <c r="BI56" s="26">
         <v>86.57</v>
       </c>
-      <c r="BJ56" s="26"/>
-      <c r="BK56" s="26"/>
+      <c r="BJ56" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK56" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL56" s="26"/>
       <c r="BM56" s="26"/>
       <c r="BN56" s="26"/>
@@ -12265,7 +12475,7 @@
         <v>18</v>
       </c>
       <c r="B57" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C57" s="26">
         <v>99.29</v>
@@ -12444,8 +12654,12 @@
       <c r="BI57" s="26">
         <v>101.51</v>
       </c>
-      <c r="BJ57" s="26"/>
-      <c r="BK57" s="26"/>
+      <c r="BJ57" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK57" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL57" s="26"/>
       <c r="BM57" s="26"/>
       <c r="BN57" s="26"/>
@@ -12468,7 +12682,7 @@
         <v>18</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C58" s="26">
         <v>96.89</v>
@@ -12647,8 +12861,12 @@
       <c r="BI58" s="26">
         <v>92.35</v>
       </c>
-      <c r="BJ58" s="26"/>
-      <c r="BK58" s="26"/>
+      <c r="BJ58" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK58" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL58" s="26"/>
       <c r="BM58" s="26"/>
       <c r="BN58" s="26"/>
@@ -12671,7 +12889,7 @@
         <v>18</v>
       </c>
       <c r="B59" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C59" s="26">
         <v>101.11</v>
@@ -12850,8 +13068,12 @@
       <c r="BI59" s="26">
         <v>95.77</v>
       </c>
-      <c r="BJ59" s="26"/>
-      <c r="BK59" s="26"/>
+      <c r="BJ59" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK59" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL59" s="26"/>
       <c r="BM59" s="26"/>
       <c r="BN59" s="26"/>
@@ -12874,7 +13096,7 @@
         <v>0</v>
       </c>
       <c r="B60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="26">
         <v>94.83</v>
@@ -13053,8 +13275,12 @@
       <c r="BI60" s="26">
         <v>88.96</v>
       </c>
-      <c r="BJ60" s="26"/>
-      <c r="BK60" s="26"/>
+      <c r="BJ60" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK60" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL60" s="26"/>
       <c r="BM60" s="26"/>
       <c r="BN60" s="26"/>
@@ -13077,7 +13303,7 @@
         <v>0</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C61" s="26">
         <v>93.06</v>
@@ -13256,8 +13482,12 @@
       <c r="BI61" s="26">
         <v>87.09</v>
       </c>
-      <c r="BJ61" s="26"/>
-      <c r="BK61" s="26"/>
+      <c r="BJ61" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK61" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL61" s="26"/>
       <c r="BM61" s="26"/>
       <c r="BN61" s="26"/>
@@ -13280,7 +13510,7 @@
         <v>0</v>
       </c>
       <c r="B62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C62" s="26">
         <v>99.29</v>
@@ -13459,8 +13689,12 @@
       <c r="BI62" s="26">
         <v>89.88</v>
       </c>
-      <c r="BJ62" s="26"/>
-      <c r="BK62" s="26"/>
+      <c r="BJ62" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK62" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL62" s="26"/>
       <c r="BM62" s="26"/>
       <c r="BN62" s="26"/>
@@ -13483,7 +13717,7 @@
         <v>0</v>
       </c>
       <c r="B63" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C63" s="26">
         <v>95.31</v>
@@ -13662,8 +13896,12 @@
       <c r="BI63" s="26">
         <v>93.29</v>
       </c>
-      <c r="BJ63" s="26"/>
-      <c r="BK63" s="26"/>
+      <c r="BJ63" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK63" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL63" s="26"/>
       <c r="BM63" s="26"/>
       <c r="BN63" s="26"/>
@@ -13686,7 +13924,7 @@
         <v>0</v>
       </c>
       <c r="B64" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C64" s="26">
         <v>99.22</v>
@@ -13865,8 +14103,12 @@
       <c r="BI64" s="26">
         <v>92.21</v>
       </c>
-      <c r="BJ64" s="26"/>
-      <c r="BK64" s="26"/>
+      <c r="BJ64" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK64" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL64" s="26"/>
       <c r="BM64" s="26"/>
       <c r="BN64" s="26"/>
@@ -13889,7 +14131,7 @@
         <v>0</v>
       </c>
       <c r="B65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C65" s="26">
         <v>96.06</v>
@@ -14068,8 +14310,12 @@
       <c r="BI65" s="26">
         <v>104.56</v>
       </c>
-      <c r="BJ65" s="26"/>
-      <c r="BK65" s="26"/>
+      <c r="BJ65" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK65" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL65" s="26"/>
       <c r="BM65" s="26"/>
       <c r="BN65" s="26"/>
@@ -14092,7 +14338,7 @@
         <v>0</v>
       </c>
       <c r="B66" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C66" s="26">
         <v>96.64</v>
@@ -14271,8 +14517,12 @@
       <c r="BI66" s="26">
         <v>98.48</v>
       </c>
-      <c r="BJ66" s="26"/>
-      <c r="BK66" s="26"/>
+      <c r="BJ66" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK66" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL66" s="26"/>
       <c r="BM66" s="26"/>
       <c r="BN66" s="26"/>
@@ -14295,7 +14545,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C67" s="26">
         <v>97.88</v>
@@ -14474,8 +14724,12 @@
       <c r="BI67" s="26">
         <v>108.02</v>
       </c>
-      <c r="BJ67" s="26"/>
-      <c r="BK67" s="26"/>
+      <c r="BJ67" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK67" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL67" s="26"/>
       <c r="BM67" s="26"/>
       <c r="BN67" s="26"/>
@@ -14498,7 +14752,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C68" s="26">
         <v>97.27</v>
@@ -14677,8 +14931,12 @@
       <c r="BI68" s="26">
         <v>96.45</v>
       </c>
-      <c r="BJ68" s="26"/>
-      <c r="BK68" s="26"/>
+      <c r="BJ68" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK68" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL68" s="26"/>
       <c r="BM68" s="26"/>
       <c r="BN68" s="26"/>
@@ -14701,7 +14959,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C69" s="26">
         <v>97.11</v>
@@ -14880,8 +15138,12 @@
       <c r="BI69" s="26">
         <v>106.03</v>
       </c>
-      <c r="BJ69" s="26"/>
-      <c r="BK69" s="26"/>
+      <c r="BJ69" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK69" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL69" s="26"/>
       <c r="BM69" s="26"/>
       <c r="BN69" s="26"/>
@@ -14904,7 +15166,7 @@
         <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="26">
         <v>92.52</v>
@@ -15083,8 +15345,12 @@
       <c r="BI70" s="26">
         <v>101.03</v>
       </c>
-      <c r="BJ70" s="26"/>
-      <c r="BK70" s="26"/>
+      <c r="BJ70" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK70" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL70" s="26"/>
       <c r="BM70" s="26"/>
       <c r="BN70" s="26"/>
@@ -15107,7 +15373,7 @@
         <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71" s="26">
         <v>93.23</v>
@@ -15286,8 +15552,12 @@
       <c r="BI71" s="26">
         <v>91.38</v>
       </c>
-      <c r="BJ71" s="26"/>
-      <c r="BK71" s="26"/>
+      <c r="BJ71" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK71" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL71" s="26"/>
       <c r="BM71" s="26"/>
       <c r="BN71" s="26"/>
@@ -15310,7 +15580,7 @@
         <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" s="26">
         <v>91.52</v>
@@ -15489,8 +15759,12 @@
       <c r="BI72" s="26">
         <v>97.18</v>
       </c>
-      <c r="BJ72" s="26"/>
-      <c r="BK72" s="26"/>
+      <c r="BJ72" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK72" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL72" s="26"/>
       <c r="BM72" s="26"/>
       <c r="BN72" s="26"/>
@@ -15513,7 +15787,7 @@
         <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73" s="26">
         <v>96.37</v>
@@ -15692,8 +15966,12 @@
       <c r="BI73" s="26">
         <v>95.8</v>
       </c>
-      <c r="BJ73" s="26"/>
-      <c r="BK73" s="26"/>
+      <c r="BJ73" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK73" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL73" s="26"/>
       <c r="BM73" s="26"/>
       <c r="BN73" s="26"/>
@@ -15716,7 +15994,7 @@
         <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74" s="26">
         <v>87.9</v>
@@ -15895,8 +16173,12 @@
       <c r="BI74" s="26">
         <v>98.7</v>
       </c>
-      <c r="BJ74" s="26"/>
-      <c r="BK74" s="26"/>
+      <c r="BJ74" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK74" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL74" s="26"/>
       <c r="BM74" s="26"/>
       <c r="BN74" s="26"/>
@@ -15919,7 +16201,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C75" s="26">
         <v>88.9</v>
@@ -16098,8 +16380,12 @@
       <c r="BI75" s="26">
         <v>92.24</v>
       </c>
-      <c r="BJ75" s="26"/>
-      <c r="BK75" s="26"/>
+      <c r="BJ75" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK75" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL75" s="26"/>
       <c r="BM75" s="26"/>
       <c r="BN75" s="26"/>
@@ -16122,7 +16408,7 @@
         <v>5</v>
       </c>
       <c r="B76" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" s="26">
         <v>95.99</v>
@@ -16301,8 +16587,12 @@
       <c r="BI76" s="26">
         <v>107</v>
       </c>
-      <c r="BJ76" s="26"/>
-      <c r="BK76" s="26"/>
+      <c r="BJ76" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK76" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL76" s="26"/>
       <c r="BM76" s="26"/>
       <c r="BN76" s="26"/>
@@ -16325,7 +16615,7 @@
         <v>5</v>
       </c>
       <c r="B77" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="26">
         <v>97.37</v>
@@ -16504,8 +16794,12 @@
       <c r="BI77" s="26">
         <v>101.35</v>
       </c>
-      <c r="BJ77" s="26"/>
-      <c r="BK77" s="26"/>
+      <c r="BJ77" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK77" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL77" s="26"/>
       <c r="BM77" s="26"/>
       <c r="BN77" s="26"/>
@@ -16528,7 +16822,7 @@
         <v>6</v>
       </c>
       <c r="B78" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" s="26">
         <v>86.12</v>
@@ -16707,8 +17001,12 @@
       <c r="BI78" s="26">
         <v>92.43</v>
       </c>
-      <c r="BJ78" s="26"/>
-      <c r="BK78" s="26"/>
+      <c r="BJ78" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK78" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL78" s="26"/>
       <c r="BM78" s="26"/>
       <c r="BN78" s="26"/>
@@ -16731,7 +17029,7 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="26">
         <v>83.5</v>
@@ -16910,8 +17208,12 @@
       <c r="BI79" s="26">
         <v>87.69</v>
       </c>
-      <c r="BJ79" s="26"/>
-      <c r="BK79" s="26"/>
+      <c r="BJ79" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK79" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL79" s="26"/>
       <c r="BM79" s="26"/>
       <c r="BN79" s="26"/>
@@ -16934,7 +17236,7 @@
         <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" s="26">
         <v>61.52</v>
@@ -17113,8 +17415,12 @@
       <c r="BI80" s="26">
         <v>89.95</v>
       </c>
-      <c r="BJ80" s="26"/>
-      <c r="BK80" s="26"/>
+      <c r="BJ80" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK80" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL80" s="26"/>
       <c r="BM80" s="26"/>
       <c r="BN80" s="26"/>
@@ -17137,7 +17443,7 @@
         <v>7</v>
       </c>
       <c r="B81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" s="26">
         <v>95.99</v>
@@ -17316,8 +17622,12 @@
       <c r="BI81" s="26">
         <v>104.62</v>
       </c>
-      <c r="BJ81" s="26"/>
-      <c r="BK81" s="26"/>
+      <c r="BJ81" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK81" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL81" s="26"/>
       <c r="BM81" s="26"/>
       <c r="BN81" s="26"/>
@@ -17340,7 +17650,7 @@
         <v>7</v>
       </c>
       <c r="B82" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" s="26">
         <v>92.34</v>
@@ -17519,8 +17829,12 @@
       <c r="BI82" s="26">
         <v>103.03</v>
       </c>
-      <c r="BJ82" s="26"/>
-      <c r="BK82" s="26"/>
+      <c r="BJ82" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK82" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL82" s="26"/>
       <c r="BM82" s="26"/>
       <c r="BN82" s="26"/>
@@ -17543,7 +17857,7 @@
         <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83" s="26">
         <v>99.84</v>
@@ -17722,8 +18036,12 @@
       <c r="BI83" s="26">
         <v>99.99</v>
       </c>
-      <c r="BJ83" s="26"/>
-      <c r="BK83" s="26"/>
+      <c r="BJ83" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK83" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL83" s="26"/>
       <c r="BM83" s="26"/>
       <c r="BN83" s="26"/>
@@ -17746,7 +18064,7 @@
         <v>7</v>
       </c>
       <c r="B84" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" s="26">
         <v>92.59</v>
@@ -17925,8 +18243,12 @@
       <c r="BI84" s="26">
         <v>106.8</v>
       </c>
-      <c r="BJ84" s="26"/>
-      <c r="BK84" s="26"/>
+      <c r="BJ84" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK84" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL84" s="26"/>
       <c r="BM84" s="26"/>
       <c r="BN84" s="26"/>
@@ -17949,7 +18271,7 @@
         <v>8</v>
       </c>
       <c r="B85" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C85" s="26">
         <v>104.01</v>
@@ -18128,8 +18450,12 @@
       <c r="BI85" s="26">
         <v>101.07</v>
       </c>
-      <c r="BJ85" s="26"/>
-      <c r="BK85" s="26"/>
+      <c r="BJ85" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK85" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL85" s="26"/>
       <c r="BM85" s="26"/>
       <c r="BN85" s="26"/>
@@ -18152,7 +18478,7 @@
         <v>8</v>
       </c>
       <c r="B86" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" s="26">
         <v>83.66</v>
@@ -18331,8 +18657,12 @@
       <c r="BI86" s="26">
         <v>91.97</v>
       </c>
-      <c r="BJ86" s="26"/>
-      <c r="BK86" s="26"/>
+      <c r="BJ86" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK86" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL86" s="26"/>
       <c r="BM86" s="26"/>
       <c r="BN86" s="26"/>
@@ -18355,7 +18685,7 @@
         <v>8</v>
       </c>
       <c r="B87" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C87" s="26">
         <v>91.08</v>
@@ -18534,8 +18864,12 @@
       <c r="BI87" s="26">
         <v>96.59</v>
       </c>
-      <c r="BJ87" s="26"/>
-      <c r="BK87" s="26"/>
+      <c r="BJ87" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK87" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL87" s="26"/>
       <c r="BM87" s="26"/>
       <c r="BN87" s="26"/>
@@ -18558,7 +18892,7 @@
         <v>8</v>
       </c>
       <c r="B88" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C88" s="26">
         <v>99.29</v>
@@ -18737,8 +19071,12 @@
       <c r="BI88" s="26">
         <v>93.61</v>
       </c>
-      <c r="BJ88" s="26"/>
-      <c r="BK88" s="26"/>
+      <c r="BJ88" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK88" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL88" s="26"/>
       <c r="BM88" s="26"/>
       <c r="BN88" s="26"/>
@@ -18761,7 +19099,7 @@
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C89" s="26">
         <v>91.06</v>
@@ -18940,8 +19278,12 @@
       <c r="BI89" s="26">
         <v>96.76</v>
       </c>
-      <c r="BJ89" s="26"/>
-      <c r="BK89" s="26"/>
+      <c r="BJ89" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK89" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL89" s="26"/>
       <c r="BM89" s="26"/>
       <c r="BN89" s="26"/>
@@ -18964,7 +19306,7 @@
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="26">
         <v>91.49</v>
@@ -19143,8 +19485,12 @@
       <c r="BI90" s="26">
         <v>96.15</v>
       </c>
-      <c r="BJ90" s="26"/>
-      <c r="BK90" s="26"/>
+      <c r="BJ90" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK90" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL90" s="26"/>
       <c r="BM90" s="26"/>
       <c r="BN90" s="26"/>
@@ -19167,7 +19513,7 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C91" s="26">
         <v>88.39</v>
@@ -19346,8 +19692,12 @@
       <c r="BI91" s="26">
         <v>99.87</v>
       </c>
-      <c r="BJ91" s="26"/>
-      <c r="BK91" s="26"/>
+      <c r="BJ91" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="BK91" s="27" t="s">
+        <v>116</v>
+      </c>
       <c r="BL91" s="26"/>
       <c r="BM91" s="26"/>
       <c r="BN91" s="26"/>
@@ -19367,7 +19717,7 @@
     </row>
     <row r="93" spans="1:79" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>